<commit_message>
Adding the economic index formater
- Adding the economic indexer formater classes
- Adding the 'dataframe_filter.py' file
- Changing some Private/Public laws
- Fixing some treeview float/int formats
- Changing the 'PORTFOLIO_TEMPLATE.xlsx' file to the discussed format
- Adapting the 'portfolio_formater.py' to the new 'PORTFOLIO_TEMPLATE.xlsx' format
- Removing unnecessary files:
  > 'vs' folder
  > calculoSelic.py
  > graphic.py
  > graphics.py
  > Investment_Portfolio_Analysis.py
  > Investment_Portfolio_Analysis.ipynb
- Code comments improvements
</commit_message>
<xml_diff>
--- a/PORTFOLIO_TEMPLATE.xlsx
+++ b/PORTFOLIO_TEMPLATE.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Extrato" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$O$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$32</definedName>
     <definedName name="Aplica">#REF!</definedName>
     <definedName name="CDI">#REF!</definedName>
     <definedName name="IR0.0">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>Data</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Custo Total</t>
   </si>
   <si>
-    <t>Líquido Total</t>
-  </si>
-  <si>
-    <t>Objetivo</t>
-  </si>
-  <si>
     <t>Custodia</t>
   </si>
   <si>
@@ -153,12 +147,6 @@
     <t>Opções</t>
   </si>
   <si>
-    <t>Aprender a operar opções</t>
-  </si>
-  <si>
-    <t>Aprender Venda Coberta</t>
-  </si>
-  <si>
     <t>PETRL19</t>
   </si>
   <si>
@@ -184,6 +172,27 @@
   </si>
   <si>
     <t>CDI</t>
+  </si>
+  <si>
+    <t>Dividendos</t>
+  </si>
+  <si>
+    <t>JCP</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Abertura de operação "Comprada"</t>
+  </si>
+  <si>
+    <t>Fechamento de operação "Comprada"</t>
+  </si>
+  <si>
+    <t>Abertura de operação "Vendida"</t>
+  </si>
+  <si>
+    <t>Fechamento de operação "Vendida" (expirada)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +203,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,12 +222,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,7 +282,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,9 +305,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -312,128 +312,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -709,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -723,11 +602,11 @@
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="50.7109375" customWidth="1"/>
+    <col min="4" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,13 +617,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -764,31 +643,34 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>41961</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="6">
         <v>1</v>
@@ -807,30 +689,32 @@
         <v>0</v>
       </c>
       <c r="M2" s="7">
-        <f t="shared" ref="M2:M10" si="1">K2+L2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7">
+        <f t="shared" ref="O2:O10" si="1">K2+L2</f>
         <v>10</v>
       </c>
-      <c r="N2" s="8">
-        <f>IF(OR(G2="Compra", G2="Resgate"),ROUNDDOWN(((J2+M2)*-1),2),ROUNDDOWN((J2-M2),2))</f>
-        <v>1000</v>
-      </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>41964</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3" s="6">
         <v>100</v>
@@ -849,36 +733,38 @@
         <v>0</v>
       </c>
       <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="N3" s="8">
-        <f t="shared" ref="N3:N10" si="2">IF(OR(G3="Compra", G3="Resgate"),ROUNDDOWN(((J3+M3)*-1),2),ROUNDDOWN((J3-M3),2))</f>
-        <v>-1010</v>
-      </c>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>41967</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4">
+        <v>43101</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.12520000000000001</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.12520000000000001</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="4">
-        <v>43101</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="6">
         <v>2</v>
@@ -897,36 +783,38 @@
         <v>0</v>
       </c>
       <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N4" s="8">
-        <f t="shared" si="2"/>
-        <v>-2005</v>
-      </c>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>41971</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43600</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5.5899999999999998E-2</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4">
-        <v>43600</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="6">
         <v>2</v>
@@ -945,30 +833,32 @@
         <v>0</v>
       </c>
       <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N5" s="8">
-        <f t="shared" si="2"/>
-        <v>-2005</v>
-      </c>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42039</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -987,78 +877,82 @@
         <v>0</v>
       </c>
       <c r="M6" s="7">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0</v>
+      </c>
+      <c r="O6" s="7">
         <f t="shared" si="1"/>
         <v>9.8000000000000007</v>
       </c>
-      <c r="N6" s="8">
-        <f t="shared" si="2"/>
-        <v>-9.8000000000000007</v>
-      </c>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>42045</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
         <v>100</v>
       </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N7" s="8">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>42103</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44256</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44256</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="6">
         <v>2</v>
@@ -1077,30 +971,32 @@
         <v>0</v>
       </c>
       <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="N8" s="8">
-        <f t="shared" si="2"/>
-        <v>-2005</v>
-      </c>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>42107</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" s="6">
         <v>100</v>
@@ -1119,30 +1015,32 @@
         <v>0</v>
       </c>
       <c r="M9" s="7">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="N9" s="8">
-        <f t="shared" si="2"/>
-        <v>1490</v>
-      </c>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>42111</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H10" s="6">
         <v>100</v>
@@ -1161,30 +1059,32 @@
         <v>50</v>
       </c>
       <c r="M10" s="7">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="N10" s="8">
-        <f t="shared" si="2"/>
-        <v>1440</v>
-      </c>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>42205</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" s="6">
         <v>1</v>
@@ -1193,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:J16" si="3">H11*I11</f>
+        <f t="shared" ref="J11:J16" si="2">H11*I11</f>
         <v>0</v>
       </c>
       <c r="K11" s="7">
@@ -1203,30 +1103,32 @@
         <v>0</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" ref="M11:M16" si="4">K11+L11</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" ref="O11:O16" si="3">K11+L11</f>
         <v>56.96</v>
       </c>
-      <c r="N11" s="8">
-        <f t="shared" ref="N11:N16" si="5">IF(OR(G11="Compra", G11="Resgate"),ROUNDDOWN(((J11+M11)*-1),2),ROUNDDOWN((J11-M11),2))</f>
-        <v>-56.96</v>
-      </c>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>42244</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H12" s="6">
         <v>100</v>
@@ -1235,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K12" s="7">
@@ -1245,32 +1147,34 @@
         <v>0</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N12" s="8">
-        <f t="shared" si="5"/>
-        <v>-210</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>42278</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H13" s="6">
         <v>100</v>
@@ -1279,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K13" s="7">
@@ -1289,32 +1193,34 @@
         <v>0</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N13" s="8">
-        <f t="shared" si="5"/>
-        <v>190</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>42326</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H14" s="6">
         <v>100</v>
@@ -1323,7 +1229,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>200</v>
       </c>
       <c r="K14" s="7">
@@ -1333,32 +1239,34 @@
         <v>0</v>
       </c>
       <c r="M14" s="7">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="N14" s="8">
-        <f t="shared" si="5"/>
-        <v>190</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>42359</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H15" s="6">
         <v>100</v>
@@ -1367,40 +1275,44 @@
         <v>0</v>
       </c>
       <c r="J15" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K15" s="7">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0</v>
-      </c>
-      <c r="M15" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>42387</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H16" s="6">
         <v>1</v>
@@ -1409,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K16" s="7">
@@ -1419,36 +1331,38 @@
         <v>0</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
+        <f t="shared" si="3"/>
         <v>147.56</v>
       </c>
-      <c r="N16" s="8">
-        <f t="shared" si="5"/>
-        <v>-147.56</v>
-      </c>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>42625</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="5">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4">
+        <v>46388</v>
+      </c>
+      <c r="E17" s="5">
         <v>0.1216</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="4">
-        <v>46388</v>
+      <c r="F17" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H17" s="6">
         <v>2</v>
@@ -1457,7 +1371,7 @@
         <v>1000</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:J22" si="6">H17*I17</f>
+        <f t="shared" ref="J17:J22" si="4">H17*I17</f>
         <v>2000</v>
       </c>
       <c r="K17" s="7">
@@ -1467,36 +1381,38 @@
         <v>0</v>
       </c>
       <c r="M17" s="7">
-        <f t="shared" ref="M17:M22" si="7">K17+L17</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <f t="shared" ref="O17:O22" si="5">K17+L17</f>
         <v>5</v>
       </c>
-      <c r="N17" s="8">
-        <f t="shared" ref="N17:N22" si="8">IF(OR(G17="Compra", G17="Resgate"),ROUNDDOWN(((J17+M17)*-1),2),ROUNDDOWN((J17-M17),2))</f>
-        <v>-2005</v>
-      </c>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>42625</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5">
+        <v>39</v>
+      </c>
+      <c r="D18" s="4">
+        <v>49444</v>
+      </c>
+      <c r="E18" s="5">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="4">
-        <v>49444</v>
+      <c r="F18" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H18" s="6">
         <v>2</v>
@@ -1505,7 +1421,7 @@
         <v>1000</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2000</v>
       </c>
       <c r="K18" s="7">
@@ -1515,40 +1431,42 @@
         <v>0</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="N18" s="8">
-        <f t="shared" si="8"/>
-        <v>-2005</v>
-      </c>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>42737</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H19" s="6">
         <v>1</v>
       </c>
       <c r="I19" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J19" s="7">
-        <f t="shared" si="6"/>
-        <v>100</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K19" s="7">
         <v>5</v>
@@ -1557,30 +1475,32 @@
         <v>10</v>
       </c>
       <c r="M19" s="7">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="7">
+        <v>100</v>
+      </c>
+      <c r="O19" s="7">
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="N19" s="8">
-        <f t="shared" si="8"/>
-        <v>85</v>
-      </c>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>42751</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H20" s="6">
         <v>1</v>
@@ -1589,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K20" s="7">
@@ -1599,36 +1519,38 @@
         <v>0</v>
       </c>
       <c r="M20" s="7">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" si="5"/>
         <v>259.8</v>
       </c>
-      <c r="N20" s="8">
-        <f t="shared" si="8"/>
-        <v>-259.8</v>
-      </c>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>42795</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="4">
+        <v>43101</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.12520000000000001</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.12520000000000001</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="4">
-        <v>43101</v>
-      </c>
       <c r="G21" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H21" s="6">
         <v>1</v>
@@ -1637,7 +1559,7 @@
         <v>850</v>
       </c>
       <c r="J21" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>850</v>
       </c>
       <c r="K21" s="7">
@@ -1647,36 +1569,38 @@
         <v>400</v>
       </c>
       <c r="M21" s="7">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0</v>
+      </c>
+      <c r="O21" s="7">
+        <f t="shared" si="5"/>
         <v>410</v>
       </c>
-      <c r="N21" s="8">
-        <f t="shared" si="8"/>
-        <v>440</v>
-      </c>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>42795</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4">
+        <v>44256</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="4">
-        <v>44256</v>
-      </c>
       <c r="G22" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H22" s="6">
         <v>1</v>
@@ -1685,7 +1609,7 @@
         <v>850</v>
       </c>
       <c r="J22" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>850</v>
       </c>
       <c r="K22" s="7">
@@ -1695,30 +1619,32 @@
         <v>100</v>
       </c>
       <c r="M22" s="7">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="7">
+        <v>0</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="N22" s="8">
-        <f t="shared" si="8"/>
-        <v>740</v>
-      </c>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>42800</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H23" s="6">
         <v>1</v>
@@ -1727,7 +1653,7 @@
         <v>5000</v>
       </c>
       <c r="J23" s="7">
-        <f t="shared" ref="J23:J25" si="9">H23*I23</f>
+        <f t="shared" ref="J23:J25" si="6">H23*I23</f>
         <v>5000</v>
       </c>
       <c r="K23" s="7">
@@ -1737,36 +1663,38 @@
         <v>0</v>
       </c>
       <c r="M23" s="7">
-        <f t="shared" ref="M23:M25" si="10">K23+L23</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="8">
-        <f t="shared" ref="N23:N25" si="11">IF(OR(G23="Compra", G23="Resgate"),ROUNDDOWN(((J23+M23)*-1),2),ROUNDDOWN((J23-M23),2))</f>
-        <v>-5000</v>
-      </c>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N23" s="7">
+        <v>0</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" ref="O23:O25" si="7">K23+L23</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43600</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43600</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="5">
-        <v>5.5899999999999998E-2</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="4">
-        <v>43600</v>
-      </c>
       <c r="G24" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H24" s="6">
         <v>4</v>
@@ -1775,7 +1703,7 @@
         <v>850</v>
       </c>
       <c r="J24" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>3400</v>
       </c>
       <c r="K24" s="7">
@@ -1785,36 +1713,38 @@
         <v>900</v>
       </c>
       <c r="M24" s="7">
-        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0</v>
+      </c>
+      <c r="O24" s="7">
+        <f t="shared" si="7"/>
         <v>910</v>
       </c>
-      <c r="N24" s="8">
-        <f t="shared" si="11"/>
-        <v>2490</v>
-      </c>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43724</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4">
+        <v>46388</v>
+      </c>
+      <c r="E25" s="5">
         <v>0.1216</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="4">
-        <v>46388</v>
+      <c r="F25" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H25" s="6">
         <v>2</v>
@@ -1823,7 +1753,7 @@
         <v>850</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>1700</v>
       </c>
       <c r="K25" s="7">
@@ -1833,36 +1763,38 @@
         <v>80</v>
       </c>
       <c r="M25" s="7">
-        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="7">
+        <v>0</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="N25" s="8">
-        <f t="shared" si="11"/>
-        <v>1610</v>
-      </c>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44312</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="5">
+        <v>42</v>
+      </c>
+      <c r="D26" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E26" s="5">
         <v>1.5</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="4">
-        <v>45042</v>
+      <c r="F26" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H26" s="6">
         <v>1000</v>
@@ -1871,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="7">
-        <f t="shared" ref="J26:J28" si="12">H26*I26</f>
+        <f t="shared" ref="J26:J28" si="8">H26*I26</f>
         <v>1000</v>
       </c>
       <c r="K26" s="7">
@@ -1881,36 +1813,38 @@
         <v>0</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" ref="M26:M28" si="13">K26+L26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
+        <v>0</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" ref="O26:O28" si="9">K26+L26</f>
         <v>5</v>
       </c>
-      <c r="N26" s="8">
-        <f t="shared" ref="N26:N28" si="14">IF(OR(G26="Compra", G26="Resgate"),ROUNDDOWN(((J26+M26)*-1),2),ROUNDDOWN((J26-M26),2))</f>
-        <v>-1005</v>
-      </c>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44312</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="5">
+        <v>42</v>
+      </c>
+      <c r="D27" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E27" s="5">
         <v>0.06</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="4">
-        <v>45042</v>
+      <c r="F27" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H27" s="6">
         <v>1000</v>
@@ -1919,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="7">
-        <f t="shared" ref="J27" si="15">H27*I27</f>
+        <f t="shared" ref="J27" si="10">H27*I27</f>
         <v>1000</v>
       </c>
       <c r="K27" s="7">
@@ -1929,78 +1863,82 @@
         <v>0</v>
       </c>
       <c r="M27" s="7">
-        <f t="shared" ref="M27" si="16">K27+L27</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="7">
+        <v>0</v>
+      </c>
+      <c r="O27" s="7">
+        <f t="shared" ref="O27" si="11">K27+L27</f>
         <v>5</v>
       </c>
-      <c r="N27" s="8">
-        <f t="shared" ref="N27" si="17">IF(OR(G27="Compra", G27="Resgate"),ROUNDDOWN(((J27+M27)*-1),2),ROUNDDOWN((J27-M27),2))</f>
-        <v>-1005</v>
-      </c>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>44344</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H28" s="6">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>15</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
         <v>100</v>
       </c>
-      <c r="I28" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="J28" s="7">
-        <f t="shared" si="12"/>
-        <v>50</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0</v>
-      </c>
-      <c r="L28" s="7">
-        <v>10</v>
-      </c>
-      <c r="M28" s="7">
-        <f t="shared" si="13"/>
-        <v>10</v>
-      </c>
-      <c r="N28" s="8">
-        <f t="shared" si="14"/>
-        <v>40</v>
-      </c>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="7">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>44312</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="5">
+        <v>42</v>
+      </c>
+      <c r="D29" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E29" s="5">
         <v>0.03</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="4">
-        <v>45042</v>
+      <c r="F29" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H29" s="6">
         <v>1000</v>
@@ -2009,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="7">
-        <f t="shared" ref="J29:J31" si="18">H29*I29</f>
+        <f t="shared" ref="J29:J31" si="12">H29*I29</f>
         <v>1000</v>
       </c>
       <c r="K29" s="7">
@@ -2019,36 +1957,38 @@
         <v>0</v>
       </c>
       <c r="M29" s="7">
-        <f t="shared" ref="M29:M31" si="19">K29+L29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7">
+        <f t="shared" ref="O29:O31" si="13">K29+L29</f>
         <v>5</v>
       </c>
-      <c r="N29" s="8">
-        <f t="shared" ref="N29:N31" si="20">IF(OR(G29="Compra", G29="Resgate"),ROUNDDOWN(((J29+M29)*-1),2),ROUNDDOWN((J29-M29),2))</f>
-        <v>-1005</v>
-      </c>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>44312</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="5">
+        <v>42</v>
+      </c>
+      <c r="D30" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E30" s="5">
         <v>1.5</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="4">
-        <v>45042</v>
+      <c r="F30" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H30" s="6">
         <v>1000</v>
@@ -2057,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="K30" s="7">
@@ -2067,36 +2007,38 @@
         <v>0</v>
       </c>
       <c r="M30" s="7">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="8">
-        <f t="shared" si="20"/>
-        <v>1000</v>
-      </c>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7">
+        <v>0</v>
+      </c>
+      <c r="O30" s="7">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>44312</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="5">
+        <v>42</v>
+      </c>
+      <c r="D31" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E31" s="5">
         <v>0.06</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="4">
-        <v>45042</v>
+      <c r="F31" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H31" s="6">
         <v>1000</v>
@@ -2105,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>1000</v>
       </c>
       <c r="K31" s="7">
@@ -2115,36 +2057,38 @@
         <v>0</v>
       </c>
       <c r="M31" s="7">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="8">
-        <f t="shared" si="20"/>
-        <v>1000</v>
-      </c>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
+        <v>0</v>
+      </c>
+      <c r="O31" s="7">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>44312</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="5">
+        <v>42</v>
+      </c>
+      <c r="D32" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E32" s="5">
         <v>0.03</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="4">
-        <v>45042</v>
+      <c r="F32" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H32" s="6">
         <v>1000</v>
@@ -2153,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="7">
-        <f t="shared" ref="J32" si="21">H32*I32</f>
+        <f t="shared" ref="J32" si="14">H32*I32</f>
         <v>1000</v>
       </c>
       <c r="K32" s="7">
@@ -2163,65 +2107,19 @@
         <v>0</v>
       </c>
       <c r="M32" s="7">
-        <f t="shared" ref="M32" si="22">K32+L32</f>
-        <v>0</v>
-      </c>
-      <c r="N32" s="8">
-        <f t="shared" ref="N32" si="23">IF(OR(G32="Compra", G32="Resgate"),ROUNDDOWN(((J32+M32)*-1),2),ROUNDDOWN((J32-M32),2))</f>
-        <v>1000</v>
-      </c>
-      <c r="O32" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
+        <v>0</v>
+      </c>
+      <c r="O32" s="7">
+        <f t="shared" ref="O32" si="15">K32+L32</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O32"/>
-  <conditionalFormatting sqref="N28 N2:N26">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N30">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N31">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N32">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <autoFilter ref="A1:P32"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add the 'currentPortfolio' and 'currentTesouroDireto' outputs inside the Portfolio Widget
- Creating several tabs in Portfolio Widget
- Adding the 'getExtrato' in 'portfolio_investment.py'
- Small fixes in 'portfolio_investment.py'
- Updating the PORTFOLIO_TEMPLATE.xlsx for testing purpose
- Removing unnecessary files:
  > extrato.py
  > treeview_example.py
  > treeview_pandas_example.py
</commit_message>
<xml_diff>
--- a/PORTFOLIO_TEMPLATE.xlsx
+++ b/PORTFOLIO_TEMPLATE.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Extrato" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Extrato!$A$1:$P$25</definedName>
     <definedName name="Aplica">#REF!</definedName>
     <definedName name="CDI">#REF!</definedName>
     <definedName name="IR0.0">#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
   <si>
     <t>Data</t>
   </si>
@@ -102,21 +102,9 @@
     <t>ITUB3</t>
   </si>
   <si>
-    <t>LTN - 01/JAN/2018</t>
-  </si>
-  <si>
-    <t>LTN (Tesouro Direto)</t>
-  </si>
-  <si>
     <t>PREFIXADO</t>
   </si>
   <si>
-    <t>NTNB Principal - 15/MAI/2019</t>
-  </si>
-  <si>
-    <t>NTNB Principal (Tesouro Direto)</t>
-  </si>
-  <si>
     <t>IPCA</t>
   </si>
   <si>
@@ -132,12 +120,6 @@
     <t>Venda</t>
   </si>
   <si>
-    <t>LFT - 01/MAR/2021</t>
-  </si>
-  <si>
-    <t>LFT (Tesouro Direto)</t>
-  </si>
-  <si>
     <t>SELIC</t>
   </si>
   <si>
@@ -150,27 +132,12 @@
     <t>PETRL19</t>
   </si>
   <si>
-    <t>NTNF - 01/JAN/2027</t>
-  </si>
-  <si>
-    <t>NTNF (Tesouro Direto)</t>
-  </si>
-  <si>
-    <t>NTNB - 15/MAI/2035</t>
-  </si>
-  <si>
-    <t>NTNB (Tesouro Direto)</t>
-  </si>
-  <si>
     <t>Resgate</t>
   </si>
   <si>
     <t>LC (SANTANA CFI) - 26/ABR/2023</t>
   </si>
   <si>
-    <t>LC (Renda Fixa)</t>
-  </si>
-  <si>
     <t>CDI</t>
   </si>
   <si>
@@ -193,6 +160,18 @@
   </si>
   <si>
     <t>Fechamento de operação "Vendida" (expirada)</t>
+  </si>
+  <si>
+    <t>Renda Fixa</t>
+  </si>
+  <si>
+    <t>Tesouro Direto</t>
+  </si>
+  <si>
+    <t>Tesouro SELIC 2023</t>
+  </si>
+  <si>
+    <t>Tesouro IPCA+ 2035</t>
   </si>
 </sst>
 </file>
@@ -588,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -644,16 +623,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -679,7 +658,7 @@
         <v>1010</v>
       </c>
       <c r="J2" s="7">
-        <f t="shared" ref="J2:J10" si="0">H2*I2</f>
+        <f t="shared" ref="J2:J9" si="0">H2*I2</f>
         <v>1010</v>
       </c>
       <c r="K2" s="7">
@@ -695,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="7">
-        <f t="shared" ref="O2:O10" si="1">K2+L2</f>
+        <f t="shared" ref="O2:O9" si="1">K2+L2</f>
         <v>10</v>
       </c>
       <c r="P2" s="4"/>
@@ -746,22 +725,22 @@
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>41967</v>
+        <v>41971</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="4">
+        <v>49444</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5.5899999999999998E-2</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="4">
-        <v>43101</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.12520000000000001</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
@@ -796,38 +775,32 @@
     </row>
     <row r="5" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>41971</v>
+        <v>42039</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4">
-        <v>43600</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5.5899999999999998E-2</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K5" s="7">
-        <v>5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L5" s="7">
         <v>0</v>
@@ -840,25 +813,25 @@
       </c>
       <c r="O5" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>42039</v>
+        <v>42045</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -871,101 +844,101 @@
         <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>9.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="L6" s="7">
         <v>0</v>
       </c>
       <c r="M6" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N6" s="7">
         <v>0</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" si="1"/>
-        <v>9.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>42045</v>
+        <v>42103</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4">
+        <v>44986</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="K7" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L7" s="7">
         <v>0</v>
       </c>
       <c r="M7" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N7" s="7">
         <v>0</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>42103</v>
+        <v>42107</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="4">
-        <v>44256</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="6">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="I8" s="7">
-        <v>1000</v>
+        <v>15</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="K8" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L8" s="7">
         <v>0</v>
@@ -978,16 +951,16 @@
       </c>
       <c r="O8" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>42107</v>
+        <v>42111</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
@@ -996,7 +969,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H9" s="6">
         <v>100</v>
@@ -1012,7 +985,7 @@
         <v>10</v>
       </c>
       <c r="L9" s="7">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M9" s="7">
         <v>0</v>
@@ -1022,41 +995,41 @@
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>42111</v>
+        <v>42244</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H10" s="6">
         <v>100</v>
       </c>
       <c r="I10" s="7">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" si="0"/>
-        <v>1500</v>
+        <f t="shared" ref="J10:J13" si="2">H10*I10</f>
+        <v>200</v>
       </c>
       <c r="K10" s="7">
         <v>10</v>
       </c>
       <c r="L10" s="7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -1065,39 +1038,41 @@
         <v>0</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="P10" s="4"/>
+        <f t="shared" ref="O10:O13" si="3">K10+L10</f>
+        <v>10</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>42205</v>
+        <v>42278</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H11" s="6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I11" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:J16" si="2">H11*I11</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="K11" s="7">
-        <v>56.96</v>
+        <v>10</v>
       </c>
       <c r="L11" s="7">
         <v>0</v>
@@ -1109,26 +1084,28 @@
         <v>0</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" ref="O11:O16" si="3">K11+L11</f>
-        <v>56.96</v>
-      </c>
-      <c r="P11" s="4"/>
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>42244</v>
+        <v>42326</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H12" s="6">
         <v>100</v>
@@ -1157,37 +1134,37 @@
         <v>10</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>42278</v>
+        <v>42359</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H13" s="6">
         <v>100</v>
       </c>
       <c r="I13" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="2"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="K13" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L13" s="7">
         <v>0</v>
@@ -1200,40 +1177,46 @@
       </c>
       <c r="O13" s="7">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>42326</v>
+        <v>42625</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D14" s="4">
+        <v>49444</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H14" s="6">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="I14" s="7">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="2"/>
-        <v>200</v>
+        <f t="shared" ref="J14:J16" si="4">H14*I14</f>
+        <v>2000</v>
       </c>
       <c r="K14" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L14" s="7">
         <v>0</v>
@@ -1245,41 +1228,39 @@
         <v>0</v>
       </c>
       <c r="O14" s="7">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>49</v>
-      </c>
+        <f t="shared" ref="O14:O16" si="5">K14+L14</f>
+        <v>5</v>
+      </c>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>42359</v>
+        <v>42751</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H15" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I15" s="7">
         <v>0</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K15" s="7">
-        <v>0</v>
+        <v>259.8</v>
       </c>
       <c r="L15" s="7">
         <v>0</v>
@@ -1291,44 +1272,48 @@
         <v>0</v>
       </c>
       <c r="O15" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>50</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>259.8</v>
+      </c>
+      <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>42387</v>
+        <v>42795</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44986</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="G16" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H16" s="6">
         <v>1</v>
       </c>
       <c r="I16" s="7">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>850</v>
       </c>
       <c r="K16" s="7">
-        <v>147.56</v>
+        <v>10</v>
       </c>
       <c r="L16" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M16" s="7">
         <v>0</v>
@@ -1337,45 +1322,39 @@
         <v>0</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="3"/>
-        <v>147.56</v>
+        <f t="shared" si="5"/>
+        <v>110</v>
       </c>
       <c r="P16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>42625</v>
+        <v>42800</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4">
-        <v>46388</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.1216</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H17" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="7">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" ref="J17:J22" si="4">H17*I17</f>
-        <v>2000</v>
+        <f t="shared" ref="J17:J18" si="6">H17*I17</f>
+        <v>5000</v>
       </c>
       <c r="K17" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L17" s="7">
         <v>0</v>
@@ -1387,48 +1366,48 @@
         <v>0</v>
       </c>
       <c r="O17" s="7">
-        <f t="shared" ref="O17:O22" si="5">K17+L17</f>
-        <v>5</v>
+        <f t="shared" ref="O17:O18" si="7">K17+L17</f>
+        <v>0</v>
       </c>
       <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>42625</v>
+        <v>43600</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4">
         <v>49444</v>
       </c>
       <c r="E18" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>5.5899999999999998E-2</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H18" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" s="7">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="J18" s="7">
-        <f t="shared" si="4"/>
-        <v>2000</v>
+        <f t="shared" si="6"/>
+        <v>850</v>
       </c>
       <c r="K18" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L18" s="7">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="M18" s="7">
         <v>0</v>
@@ -1437,83 +1416,95 @@
         <v>0</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="7"/>
+        <v>910</v>
       </c>
       <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>42737</v>
+        <v>44312</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G19" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H19" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I19" s="7">
         <v>1</v>
       </c>
-      <c r="I19" s="7">
-        <v>0</v>
-      </c>
       <c r="J19" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J19:J21" si="8">H19*I19</f>
+        <v>1000</v>
       </c>
       <c r="K19" s="7">
         <v>5</v>
       </c>
       <c r="L19" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M19" s="7">
         <v>0</v>
       </c>
       <c r="N19" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" ref="O19:O21" si="9">K19+L19</f>
+        <v>5</v>
       </c>
       <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>42751</v>
+        <v>44312</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G20" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H20" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I20" s="7">
         <v>1</v>
       </c>
-      <c r="I20" s="7">
-        <v>0</v>
-      </c>
       <c r="J20" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J20" si="10">H20*I20</f>
+        <v>1000</v>
       </c>
       <c r="K20" s="7">
-        <v>259.8</v>
+        <v>5</v>
       </c>
       <c r="L20" s="7">
         <v>0</v>
@@ -1525,98 +1516,92 @@
         <v>0</v>
       </c>
       <c r="O20" s="7">
-        <f t="shared" si="5"/>
-        <v>259.8</v>
+        <f t="shared" ref="O20" si="11">K20+L20</f>
+        <v>5</v>
       </c>
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>42795</v>
+        <v>44344</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="4">
-        <v>43101</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0.12520000000000001</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H21" s="6">
         <v>1</v>
       </c>
       <c r="I21" s="7">
-        <v>850</v>
+        <v>0</v>
       </c>
       <c r="J21" s="7">
-        <f t="shared" si="4"/>
-        <v>850</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="K21" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L21" s="7">
-        <v>400</v>
+        <v>15</v>
       </c>
       <c r="M21" s="7">
         <v>0</v>
       </c>
       <c r="N21" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O21" s="7">
-        <f t="shared" si="5"/>
-        <v>410</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="P21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>42795</v>
+        <v>44312</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4">
-        <v>44256</v>
+        <v>45042</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H22" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I22" s="7">
         <v>1</v>
       </c>
-      <c r="I22" s="7">
-        <v>850</v>
-      </c>
       <c r="J22" s="7">
-        <f t="shared" si="4"/>
-        <v>850</v>
+        <f t="shared" ref="J22:J24" si="12">H22*I22</f>
+        <v>1000</v>
       </c>
       <c r="K22" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L22" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M22" s="7">
         <v>0</v>
@@ -1625,36 +1610,42 @@
         <v>0</v>
       </c>
       <c r="O22" s="7">
-        <f t="shared" si="5"/>
-        <v>110</v>
+        <f t="shared" ref="O22:O24" si="13">K22+L22</f>
+        <v>5</v>
       </c>
       <c r="P22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>42800</v>
+        <v>44312</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45042</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G23" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H23" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I23" s="7">
         <v>1</v>
       </c>
-      <c r="I23" s="7">
-        <v>5000</v>
-      </c>
       <c r="J23" s="7">
-        <f t="shared" ref="J23:J25" si="6">H23*I23</f>
-        <v>5000</v>
+        <f t="shared" si="12"/>
+        <v>1000</v>
       </c>
       <c r="K23" s="7">
         <v>0</v>
@@ -1669,48 +1660,48 @@
         <v>0</v>
       </c>
       <c r="O23" s="7">
-        <f t="shared" ref="O23:O25" si="7">K23+L23</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>43600</v>
+        <v>44312</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4">
-        <v>43600</v>
+        <v>45042</v>
       </c>
       <c r="E24" s="5">
-        <v>5.5899999999999998E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="H24" s="6">
-        <v>4</v>
+        <v>1000</v>
       </c>
       <c r="I24" s="7">
-        <v>850</v>
+        <v>1</v>
       </c>
       <c r="J24" s="7">
-        <f t="shared" si="6"/>
-        <v>3400</v>
+        <f t="shared" si="12"/>
+        <v>1000</v>
       </c>
       <c r="K24" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L24" s="7">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="M24" s="7">
         <v>0</v>
@@ -1719,48 +1710,48 @@
         <v>0</v>
       </c>
       <c r="O24" s="7">
-        <f t="shared" si="7"/>
-        <v>910</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>43724</v>
+        <v>44312</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D25" s="4">
-        <v>46388</v>
+        <v>45042</v>
       </c>
       <c r="E25" s="5">
-        <v>0.1216</v>
+        <v>0.03</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H25" s="6">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="I25" s="7">
-        <v>850</v>
+        <v>1</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="6"/>
-        <v>1700</v>
+        <f t="shared" ref="J25" si="14">H25*I25</f>
+        <v>1000</v>
       </c>
       <c r="K25" s="7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L25" s="7">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M25" s="7">
         <v>0</v>
@@ -1769,357 +1760,13 @@
         <v>0</v>
       </c>
       <c r="O25" s="7">
-        <f t="shared" si="7"/>
-        <v>90</v>
+        <f t="shared" ref="O25" si="15">K25+L25</f>
+        <v>0</v>
       </c>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E26" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I26" s="7">
-        <v>1</v>
-      </c>
-      <c r="J26" s="7">
-        <f t="shared" ref="J26:J28" si="8">H26*I26</f>
-        <v>1000</v>
-      </c>
-      <c r="K26" s="7">
-        <v>5</v>
-      </c>
-      <c r="L26" s="7">
-        <v>0</v>
-      </c>
-      <c r="M26" s="7">
-        <v>0</v>
-      </c>
-      <c r="N26" s="7">
-        <v>0</v>
-      </c>
-      <c r="O26" s="7">
-        <f t="shared" ref="O26:O28" si="9">K26+L26</f>
-        <v>5</v>
-      </c>
-      <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I27" s="7">
-        <v>1</v>
-      </c>
-      <c r="J27" s="7">
-        <f t="shared" ref="J27" si="10">H27*I27</f>
-        <v>1000</v>
-      </c>
-      <c r="K27" s="7">
-        <v>5</v>
-      </c>
-      <c r="L27" s="7">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7">
-        <v>0</v>
-      </c>
-      <c r="N27" s="7">
-        <v>0</v>
-      </c>
-      <c r="O27" s="7">
-        <f t="shared" ref="O27" si="11">K27+L27</f>
-        <v>5</v>
-      </c>
-      <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>44344</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="6">
-        <v>1</v>
-      </c>
-      <c r="I28" s="7">
-        <v>0</v>
-      </c>
-      <c r="J28" s="7">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0</v>
-      </c>
-      <c r="L28" s="7">
-        <v>15</v>
-      </c>
-      <c r="M28" s="7">
-        <v>0</v>
-      </c>
-      <c r="N28" s="7">
-        <v>100</v>
-      </c>
-      <c r="O28" s="7">
-        <f t="shared" si="9"/>
-        <v>15</v>
-      </c>
-      <c r="P28" s="4"/>
-    </row>
-    <row r="29" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I29" s="7">
-        <v>1</v>
-      </c>
-      <c r="J29" s="7">
-        <f t="shared" ref="J29:J31" si="12">H29*I29</f>
-        <v>1000</v>
-      </c>
-      <c r="K29" s="7">
-        <v>5</v>
-      </c>
-      <c r="L29" s="7">
-        <v>0</v>
-      </c>
-      <c r="M29" s="7">
-        <v>0</v>
-      </c>
-      <c r="N29" s="7">
-        <v>0</v>
-      </c>
-      <c r="O29" s="7">
-        <f t="shared" ref="O29:O31" si="13">K29+L29</f>
-        <v>5</v>
-      </c>
-      <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E30" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I30" s="7">
-        <v>1</v>
-      </c>
-      <c r="J30" s="7">
-        <f t="shared" si="12"/>
-        <v>1000</v>
-      </c>
-      <c r="K30" s="7">
-        <v>0</v>
-      </c>
-      <c r="L30" s="7">
-        <v>0</v>
-      </c>
-      <c r="M30" s="7">
-        <v>0</v>
-      </c>
-      <c r="N30" s="7">
-        <v>0</v>
-      </c>
-      <c r="O30" s="7">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E31" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I31" s="7">
-        <v>1</v>
-      </c>
-      <c r="J31" s="7">
-        <f t="shared" si="12"/>
-        <v>1000</v>
-      </c>
-      <c r="K31" s="7">
-        <v>0</v>
-      </c>
-      <c r="L31" s="7">
-        <v>0</v>
-      </c>
-      <c r="M31" s="7">
-        <v>0</v>
-      </c>
-      <c r="N31" s="7">
-        <v>0</v>
-      </c>
-      <c r="O31" s="7">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>44312</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="4">
-        <v>45042</v>
-      </c>
-      <c r="E32" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="6">
-        <v>1000</v>
-      </c>
-      <c r="I32" s="7">
-        <v>1</v>
-      </c>
-      <c r="J32" s="7">
-        <f t="shared" ref="J32" si="14">H32*I32</f>
-        <v>1000</v>
-      </c>
-      <c r="K32" s="7">
-        <v>0</v>
-      </c>
-      <c r="L32" s="7">
-        <v>0</v>
-      </c>
-      <c r="M32" s="7">
-        <v>0</v>
-      </c>
-      <c r="N32" s="7">
-        <v>0</v>
-      </c>
-      <c r="O32" s="7">
-        <f t="shared" ref="O32" si="15">K32+L32</f>
-        <v>0</v>
-      </c>
-      <c r="P32" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P32"/>
+  <autoFilter ref="A1:P25"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>